<commit_message>
Enchanted book crafting complete, built new version
</commit_message>
<xml_diff>
--- a/Implementation Docs/Enchanting Books.xlsx
+++ b/Implementation Docs/Enchanting Books.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Sweeping Edge</t>
   </si>
   <si>
-    <t>Determinant</t>
-  </si>
-  <si>
     <t>Water Bottle</t>
   </si>
   <si>
@@ -135,18 +132,9 @@
     <t>Ice</t>
   </si>
   <si>
-    <t>Redstone</t>
-  </si>
-  <si>
-    <t>Feather</t>
-  </si>
-  <si>
     <t>Blaze Powder</t>
   </si>
   <si>
-    <t>Magma Cream</t>
-  </si>
-  <si>
     <t>Diamond</t>
   </si>
   <si>
@@ -168,43 +156,61 @@
     <t>Rabbit's Foot</t>
   </si>
   <si>
-    <t>Prismarine Crystal</t>
-  </si>
-  <si>
-    <t>Book</t>
-  </si>
-  <si>
-    <t>Iron</t>
-  </si>
-  <si>
-    <t>Prismarine Shard</t>
-  </si>
-  <si>
-    <t>Ghast Tear</t>
-  </si>
-  <si>
     <t>Cactus</t>
   </si>
   <si>
     <t>Rotten Flesh</t>
   </si>
   <si>
-    <t>Enchanting Book</t>
-  </si>
-  <si>
     <t>Lead</t>
   </si>
   <si>
     <t>Gunpowder</t>
   </si>
   <si>
-    <t>Nether Quartz</t>
+    <t>Advancement</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Potion of Regeneration</t>
+  </si>
+  <si>
+    <t>Potion of Strength</t>
+  </si>
+  <si>
+    <t>Potion of Swiftness</t>
+  </si>
+  <si>
+    <t>Potion of Leaping</t>
+  </si>
+  <si>
+    <t>Potion of Fire Resistance</t>
+  </si>
+  <si>
+    <t>Potion of Water Breathing</t>
+  </si>
+  <si>
+    <t>Shears</t>
+  </si>
+  <si>
+    <t>Determinant 2</t>
+  </si>
+  <si>
+    <t>Determinant 1</t>
+  </si>
+  <si>
+    <t>Iron Ingot</t>
+  </si>
+  <si>
+    <t>Prismarine Crystals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -234,13 +240,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -254,17 +279,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E31" totalsRowShown="0">
-  <autoFilter ref="A1:E31"/>
-  <sortState ref="A2:E31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F31" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:F31"/>
+  <sortState ref="A2:F31">
     <sortCondition ref="A1:A31"/>
   </sortState>
-  <tableColumns count="5">
+  <tableColumns count="6">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="3" name="ID"/>
-    <tableColumn id="9" name="Book"/>
-    <tableColumn id="7" name="Determinant"/>
-    <tableColumn id="8" name="Coded"/>
+    <tableColumn id="9" name="Determinant 1" dataDxfId="2"/>
+    <tableColumn id="7" name="Determinant 2" dataDxfId="0"/>
+    <tableColumn id="8" name="Coded" dataDxfId="1"/>
+    <tableColumn id="2" name="Advancement" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -533,7 +559,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -543,446 +569,631 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
       <c r="B6">
         <v>71</v>
       </c>
-      <c r="C6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8">
         <v>32</v>
       </c>
-      <c r="C8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
-      <c r="C9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10">
         <v>20</v>
       </c>
-      <c r="C10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="B12">
         <v>50</v>
       </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13">
         <v>35</v>
       </c>
-      <c r="C13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14">
         <v>9</v>
       </c>
-      <c r="C14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15">
         <v>51</v>
       </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16">
         <v>19</v>
       </c>
-      <c r="C16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
       <c r="B17">
         <v>21</v>
       </c>
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18">
         <v>61</v>
       </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
       <c r="B19">
         <v>62</v>
       </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
       <c r="B20">
         <v>70</v>
       </c>
-      <c r="C20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
       <c r="B21">
         <v>48</v>
       </c>
-      <c r="C21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
       <c r="B22">
         <v>4</v>
       </c>
-      <c r="C22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
-      <c r="C23" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
       <c r="B24">
         <v>49</v>
       </c>
-      <c r="C24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
       <c r="B25">
         <v>5</v>
       </c>
-      <c r="C25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
       <c r="B26">
         <v>16</v>
       </c>
-      <c r="C26" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
       <c r="B27">
         <v>33</v>
       </c>
-      <c r="C27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="C27" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
       <c r="B28">
         <v>17</v>
       </c>
-      <c r="C28" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
       <c r="B29">
         <v>22</v>
       </c>
-      <c r="C29" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
       <c r="B30">
         <v>7</v>
       </c>
-      <c r="C30" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>27</v>
       </c>
       <c r="B31">
         <v>34</v>
       </c>
-      <c r="C31" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" t="s">
-        <v>36</v>
+      <c r="C31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>